<commit_message>
Added PAR1 signaling module.
</commit_message>
<xml_diff>
--- a/Model_Parameters.xlsx
+++ b/Model_Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Alexey\anjumso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B93FE03C-2BDF-4AC4-9721-4345F93D6F69}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E5CA13D-26EC-41B3-8D54-FA7DAA2339AC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Clustering" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="LAT_Pars" sheetId="4" r:id="rId3"/>
     <sheet name="CalciumModule" sheetId="5" r:id="rId4"/>
     <sheet name="InitialConcentrations" sheetId="3" r:id="rId5"/>
+    <sheet name="PAR1" sheetId="7" r:id="rId6"/>
+    <sheet name="InitPAR1" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="221">
   <si>
     <t>Parname</t>
   </si>
@@ -419,6 +421,279 @@
   </si>
   <si>
     <t>Reverse rate of Calcium buffering</t>
+  </si>
+  <si>
+    <t>par1</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>sfllrn</t>
+  </si>
+  <si>
+    <t>par1_a</t>
+  </si>
+  <si>
+    <t>gqgtp</t>
+  </si>
+  <si>
+    <t>gqgdp</t>
+  </si>
+  <si>
+    <t>plcgqgtp</t>
+  </si>
+  <si>
+    <t>plcgqgdp</t>
+  </si>
+  <si>
+    <t>par1_gq</t>
+  </si>
+  <si>
+    <t>gtp</t>
+  </si>
+  <si>
+    <t>par1_gqgtpgdp</t>
+  </si>
+  <si>
+    <t>gdp</t>
+  </si>
+  <si>
+    <t>par1_gqgdp</t>
+  </si>
+  <si>
+    <t>plcgqgtppip2</t>
+  </si>
+  <si>
+    <t>plc</t>
+  </si>
+  <si>
+    <t>pip2</t>
+  </si>
+  <si>
+    <t>ca_ex</t>
+  </si>
+  <si>
+    <t>ip3r</t>
+  </si>
+  <si>
+    <t>orai1_closed</t>
+  </si>
+  <si>
+    <t>orai1_opened</t>
+  </si>
+  <si>
+    <t>stim1</t>
+  </si>
+  <si>
+    <t>stim1ca</t>
+  </si>
+  <si>
+    <t>ca_mit</t>
+  </si>
+  <si>
+    <t>phi</t>
+  </si>
+  <si>
+    <t>mptp_opened</t>
+  </si>
+  <si>
+    <t>mptp_closed</t>
+  </si>
+  <si>
+    <t>k4</t>
+  </si>
+  <si>
+    <t>k5</t>
+  </si>
+  <si>
+    <t>k6</t>
+  </si>
+  <si>
+    <t>k7</t>
+  </si>
+  <si>
+    <t>k8</t>
+  </si>
+  <si>
+    <t>k9</t>
+  </si>
+  <si>
+    <t>k10</t>
+  </si>
+  <si>
+    <t>k11</t>
+  </si>
+  <si>
+    <t>k12</t>
+  </si>
+  <si>
+    <t>km_1</t>
+  </si>
+  <si>
+    <t>km_2</t>
+  </si>
+  <si>
+    <t>km_3</t>
+  </si>
+  <si>
+    <t>km_4</t>
+  </si>
+  <si>
+    <t>km_5</t>
+  </si>
+  <si>
+    <t>km_6</t>
+  </si>
+  <si>
+    <t>km_7</t>
+  </si>
+  <si>
+    <t>km_8</t>
+  </si>
+  <si>
+    <t>km_9</t>
+  </si>
+  <si>
+    <t>km_10</t>
+  </si>
+  <si>
+    <t>km_11</t>
+  </si>
+  <si>
+    <t>gamma_1</t>
+  </si>
+  <si>
+    <t>gamma_2</t>
+  </si>
+  <si>
+    <t>gamma_3</t>
+  </si>
+  <si>
+    <t>gamma_4</t>
+  </si>
+  <si>
+    <t>gamma_5</t>
+  </si>
+  <si>
+    <t>gamma_6</t>
+  </si>
+  <si>
+    <t>gamma_7</t>
+  </si>
+  <si>
+    <t>gamma_8</t>
+  </si>
+  <si>
+    <t>gamma_9</t>
+  </si>
+  <si>
+    <t>gamma_10</t>
+  </si>
+  <si>
+    <t>gamma_11</t>
+  </si>
+  <si>
+    <t>V_1</t>
+  </si>
+  <si>
+    <t>V_2</t>
+  </si>
+  <si>
+    <t>K_1</t>
+  </si>
+  <si>
+    <t>K_2</t>
+  </si>
+  <si>
+    <t>K_3</t>
+  </si>
+  <si>
+    <t>k_3</t>
+  </si>
+  <si>
+    <t>k_4</t>
+  </si>
+  <si>
+    <t>k_5</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>L3</t>
+  </si>
+  <si>
+    <t>L5</t>
+  </si>
+  <si>
+    <t>K3</t>
+  </si>
+  <si>
+    <t>K5</t>
+  </si>
+  <si>
+    <t>K6</t>
+  </si>
+  <si>
+    <t>K7</t>
+  </si>
+  <si>
+    <t>K8</t>
+  </si>
+  <si>
+    <t>km2</t>
+  </si>
+  <si>
+    <t>km3</t>
+  </si>
+  <si>
+    <t>km4</t>
+  </si>
+  <si>
+    <t>kc3</t>
+  </si>
+  <si>
+    <t>k_12</t>
+  </si>
+  <si>
+    <t>k_13</t>
+  </si>
+  <si>
+    <t>phi_a1</t>
+  </si>
+  <si>
+    <t>phi_a2</t>
+  </si>
+  <si>
+    <t>phi_a3</t>
+  </si>
+  <si>
+    <t>phi_a4</t>
+  </si>
+  <si>
+    <t>phi_m</t>
+  </si>
+  <si>
+    <t>phi_m2</t>
+  </si>
+  <si>
+    <t>phi_m3</t>
+  </si>
+  <si>
+    <t>jres</t>
+  </si>
+  <si>
+    <t>k_thr</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -887,7 +1162,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5"/>
@@ -1113,7 +1388,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5"/>
@@ -1309,7 +1584,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1455,15 +1730,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3BD2B2B-8F87-46B1-8F65-9604D3DE87AA}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1471,7 +1746,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -1482,7 +1757,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>66</v>
       </c>
@@ -1493,7 +1768,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>67</v>
       </c>
@@ -1503,8 +1778,11 @@
       <c r="C4" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="E4">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>68</v>
       </c>
@@ -1515,7 +1793,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>69</v>
       </c>
@@ -1526,18 +1804,18 @@
         <v>127</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>71</v>
       </c>
       <c r="B7">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="C7" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>70</v>
       </c>
@@ -1557,8 +1835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5"/>
@@ -1579,7 +1857,10 @@
       <c r="A2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="6">
+        <v>5000</v>
+      </c>
+      <c r="C2" s="6">
         <v>1.18E-4</v>
       </c>
       <c r="D2" s="1"/>
@@ -1966,4 +2247,819 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F2972C9-1B86-49F1-91CE-527F0C1D5946}">
+  <dimension ref="A1:B71"/>
+  <sheetViews>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>157</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>158</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>160</v>
+      </c>
+      <c r="B9">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>161</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>162</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>163</v>
+      </c>
+      <c r="B12">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>164</v>
+      </c>
+      <c r="B13">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>165</v>
+      </c>
+      <c r="B14">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>166</v>
+      </c>
+      <c r="B15">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>167</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>168</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>169</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>170</v>
+      </c>
+      <c r="B19">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>171</v>
+      </c>
+      <c r="B20">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>172</v>
+      </c>
+      <c r="B21">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>173</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1.8E-5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>174</v>
+      </c>
+      <c r="B23">
+        <v>6.8000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>175</v>
+      </c>
+      <c r="B24">
+        <v>2.5350000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>176</v>
+      </c>
+      <c r="B25">
+        <v>0.113</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>177</v>
+      </c>
+      <c r="B26">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>178</v>
+      </c>
+      <c r="B27">
+        <v>420000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>179</v>
+      </c>
+      <c r="B28">
+        <v>1.55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>180</v>
+      </c>
+      <c r="B29">
+        <v>1840</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>181</v>
+      </c>
+      <c r="B30">
+        <v>64.2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>182</v>
+      </c>
+      <c r="B31">
+        <v>8.8499999999999995E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>183</v>
+      </c>
+      <c r="B32">
+        <v>1.27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>184</v>
+      </c>
+      <c r="B33">
+        <v>1.73E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>185</v>
+      </c>
+      <c r="B34">
+        <v>0.39700000000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>186</v>
+      </c>
+      <c r="B35">
+        <v>0.13800000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>187</v>
+      </c>
+      <c r="B36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>188</v>
+      </c>
+      <c r="B37">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>189</v>
+      </c>
+      <c r="B38">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>190</v>
+      </c>
+      <c r="B39">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>191</v>
+      </c>
+      <c r="B40">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41">
+        <v>11.94</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B42">
+        <v>1.78</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>192</v>
+      </c>
+      <c r="B43">
+        <v>37.4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>193</v>
+      </c>
+      <c r="B44">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>194</v>
+      </c>
+      <c r="B45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>195</v>
+      </c>
+      <c r="B46">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>196</v>
+      </c>
+      <c r="B47">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>197</v>
+      </c>
+      <c r="B48">
+        <v>54.7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>198</v>
+      </c>
+      <c r="B49">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>199</v>
+      </c>
+      <c r="B50">
+        <v>4707</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>200</v>
+      </c>
+      <c r="B51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>201</v>
+      </c>
+      <c r="B52">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>202</v>
+      </c>
+      <c r="B53">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>203</v>
+      </c>
+      <c r="B54">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>204</v>
+      </c>
+      <c r="B55">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>205</v>
+      </c>
+      <c r="B56">
+        <v>29.8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
+        <v>206</v>
+      </c>
+      <c r="B57">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
+        <v>207</v>
+      </c>
+      <c r="B58">
+        <v>1.266</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
+        <v>208</v>
+      </c>
+      <c r="B59">
+        <v>667000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>209</v>
+      </c>
+      <c r="B60">
+        <v>9.0999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" t="s">
+        <v>210</v>
+      </c>
+      <c r="B61">
+        <v>1.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
+        <v>211</v>
+      </c>
+      <c r="B62">
+        <v>9.0999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
+        <v>212</v>
+      </c>
+      <c r="B63">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
+        <v>213</v>
+      </c>
+      <c r="B64">
+        <v>0.124</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
+        <v>214</v>
+      </c>
+      <c r="B65">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
+        <v>215</v>
+      </c>
+      <c r="B66">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
+        <v>216</v>
+      </c>
+      <c r="B67">
+        <v>3.45</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" t="s">
+        <v>217</v>
+      </c>
+      <c r="B68">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" t="s">
+        <v>218</v>
+      </c>
+      <c r="B69" s="1">
+        <v>8.3099999999999997E-3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" t="s">
+        <v>219</v>
+      </c>
+      <c r="B70">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" t="s">
+        <v>220</v>
+      </c>
+      <c r="B71">
+        <v>96.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5829A873-6480-4FF2-9496-6583C6574425}">
+  <dimension ref="A1:B27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7">
+        <v>4.3E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>138</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>140</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>142</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>143</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>144</v>
+      </c>
+      <c r="B16">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>145</v>
+      </c>
+      <c r="B17">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>146</v>
+      </c>
+      <c r="B18">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>147</v>
+      </c>
+      <c r="B19">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>148</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>149</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>150</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>151</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>152</v>
+      </c>
+      <c r="B24">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>153</v>
+      </c>
+      <c r="B25">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>154</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>155</v>
+      </c>
+      <c r="B27">
+        <v>0.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changed a couple of parameters and checked overall model stability.
</commit_message>
<xml_diff>
--- a/Model_Parameters.xlsx
+++ b/Model_Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Alexey\anjumso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{837F587B-F0B5-4577-B2E9-6F3236DB8334}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44967BE8-FF6E-4616-974D-D828E74A5C57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Clustering" sheetId="1" r:id="rId1"/>
@@ -1746,7 +1746,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1848,8 +1848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5"/>
@@ -2145,7 +2145,7 @@
         <v>75</v>
       </c>
       <c r="B33" s="7">
-        <v>26.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -2278,7 +2278,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F2972C9-1B86-49F1-91CE-527F0C1D5946}">
   <dimension ref="A1:B71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Corrected DTS Calcium concentration.
</commit_message>
<xml_diff>
--- a/Model_Parameters.xlsx
+++ b/Model_Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Alexey\anjumso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44967BE8-FF6E-4616-974D-D828E74A5C57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78B0D85-4B2B-45A9-9433-F1CE3383DE9F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Clustering" sheetId="1" r:id="rId1"/>
@@ -1745,8 +1745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3BD2B2B-8F87-46B1-8F65-9604D3DE87AA}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1822,7 +1822,7 @@
         <v>71</v>
       </c>
       <c r="B7">
-        <v>0.5</v>
+        <v>1.2</v>
       </c>
       <c r="C7" t="s">
         <v>128</v>
@@ -1848,8 +1848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5"/>
@@ -2129,7 +2129,7 @@
         <v>73</v>
       </c>
       <c r="B31" s="7">
-        <v>194.52</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -2278,7 +2278,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F2972C9-1B86-49F1-91CE-527F0C1D5946}">
   <dimension ref="A1:B71"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
@@ -2861,8 +2861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5829A873-6480-4FF2-9496-6583C6574425}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
Added more convenient plotter.
</commit_message>
<xml_diff>
--- a/Model_Parameters.xlsx
+++ b/Model_Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Alexey\anjumso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78B0D85-4B2B-45A9-9433-F1CE3383DE9F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235E1091-A51F-45D3-ACE8-10B7FAA59F2B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Clustering" sheetId="1" r:id="rId1"/>
@@ -1745,7 +1745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3BD2B2B-8F87-46B1-8F65-9604D3DE87AA}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -1848,8 +1848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5"/>
@@ -2145,7 +2145,7 @@
         <v>75</v>
       </c>
       <c r="B33" s="7">
-        <v>0</v>
+        <v>26.6</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -2861,8 +2861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5829A873-6480-4FF2-9496-6583C6574425}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
Finalized the plotting module and added slider generation for PAR1 module.
</commit_message>
<xml_diff>
--- a/Model_Parameters.xlsx
+++ b/Model_Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Alexey\anjumso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235E1091-A51F-45D3-ACE8-10B7FAA59F2B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E58C22-70BE-44CB-99F9-42BDE910E5F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Clustering" sheetId="1" r:id="rId1"/>
@@ -1597,7 +1597,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1848,7 +1848,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
@@ -2278,8 +2278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F2972C9-1B86-49F1-91CE-527F0C1D5946}">
   <dimension ref="A1:B71"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
Added second plot plotter. Corrected the description for the slider generation.
</commit_message>
<xml_diff>
--- a/Model_Parameters.xlsx
+++ b/Model_Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Alexey\anjumso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E58C22-70BE-44CB-99F9-42BDE910E5F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{792B60D8-8E25-4C58-9A83-64FB226A95AC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Clustering" sheetId="1" r:id="rId1"/>
@@ -2278,7 +2278,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F2972C9-1B86-49F1-91CE-527F0C1D5946}">
   <dimension ref="A1:B71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
@@ -2861,8 +2861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5829A873-6480-4FF2-9496-6583C6574425}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>